<commit_message>
queue and queue manager should be done
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\Codegym_Module_2\Case_Study\accounting_software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFE3F56-94C1-4AE5-B87D-F5538C177102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE29DE3-D692-45AE-B5B2-DF7D2EF5BE7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{97F2DD4E-FD07-4A13-BFEB-826D5C26E65D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{97F2DD4E-FD07-4A13-BFEB-826D5C26E65D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="idea" sheetId="1" r:id="rId1"/>
+    <sheet name="shortVersion" sheetId="2" r:id="rId2"/>
+    <sheet name="156" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="109">
   <si>
     <t>Tiền mặt</t>
   </si>
@@ -260,13 +261,106 @@
   </si>
   <si>
     <t>giả sử không phải nộp thuế</t>
+  </si>
+  <si>
+    <t>Phiếu xuất kho</t>
+  </si>
+  <si>
+    <t>Phiếu nhập kho</t>
+  </si>
+  <si>
+    <t>Tên người lập</t>
+  </si>
+  <si>
+    <t>Tên sản phẩm</t>
+  </si>
+  <si>
+    <t>Ngày lập</t>
+  </si>
+  <si>
+    <t>(Tạm bỏ qua)</t>
+  </si>
+  <si>
+    <t>ID phiếu</t>
+  </si>
+  <si>
+    <t>Số lượng</t>
+  </si>
+  <si>
+    <t>giá nhập</t>
+  </si>
+  <si>
+    <t>giá bán</t>
+  </si>
+  <si>
+    <t>&gt;&gt;&gt;</t>
+  </si>
+  <si>
+    <t>Set giá bán sau khi tạo phiếu nhập kho</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>Nhập tay</t>
+  </si>
+  <si>
+    <t>Auto</t>
+  </si>
+  <si>
+    <t>Lý do xuất</t>
+  </si>
+  <si>
+    <t>Lý do nhập</t>
+  </si>
+  <si>
+    <t>Lấy từ giá set ở trên</t>
+  </si>
+  <si>
+    <t>&gt;&gt;&gt; Lập bút toán</t>
+  </si>
+  <si>
+    <t>Tăng 156</t>
+  </si>
+  <si>
+    <t>Giảm 111</t>
+  </si>
+  <si>
+    <t>giảm 156</t>
+  </si>
+  <si>
+    <t>tăng 111</t>
+  </si>
+  <si>
+    <t>tăng 632</t>
+  </si>
+  <si>
+    <t>số lượng x giá nhập</t>
+  </si>
+  <si>
+    <t>tính theo phương pháp fifo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tăng 515 </t>
+  </si>
+  <si>
+    <t>và</t>
+  </si>
+  <si>
+    <t>switchcase&gt;&gt;&gt;&gt;</t>
+  </si>
+  <si>
+    <t>hoặc giá bán = 0</t>
+  </si>
+  <si>
+    <t>hàng hỏng/ lý do khác</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,6 +372,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -318,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -326,6 +427,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -998,7 +1100,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{989E85F1-71CC-4157-9970-ADAF606AA44C}">
   <dimension ref="C3:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -1147,4 +1249,195 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2859D1AD-D06B-4526-AF9E-F8462D477E43}">
+  <dimension ref="B5:Q17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.21875" customWidth="1"/>
+    <col min="14" max="14" width="26" customWidth="1"/>
+    <col min="15" max="15" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="C5" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I6" t="s">
+        <v>82</v>
+      </c>
+      <c r="J6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" t="s">
+        <v>91</v>
+      </c>
+      <c r="I7" t="s">
+        <v>84</v>
+      </c>
+      <c r="J7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" t="s">
+        <v>91</v>
+      </c>
+      <c r="I8" t="s">
+        <v>94</v>
+      </c>
+      <c r="J8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F9" t="s">
+        <v>91</v>
+      </c>
+      <c r="N9" t="s">
+        <v>97</v>
+      </c>
+      <c r="O9" t="s">
+        <v>98</v>
+      </c>
+      <c r="P9" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G10" t="s">
+        <v>91</v>
+      </c>
+      <c r="L10" t="s">
+        <v>96</v>
+      </c>
+      <c r="N10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" ht="45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="C12" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" t="s">
+        <v>90</v>
+      </c>
+      <c r="I13" t="s">
+        <v>82</v>
+      </c>
+      <c r="J13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" t="s">
+        <v>91</v>
+      </c>
+      <c r="I14" t="s">
+        <v>84</v>
+      </c>
+      <c r="J14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>85</v>
+      </c>
+      <c r="F15" t="s">
+        <v>91</v>
+      </c>
+      <c r="I15" t="s">
+        <v>93</v>
+      </c>
+      <c r="J15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" t="s">
+        <v>95</v>
+      </c>
+      <c r="L16" t="s">
+        <v>96</v>
+      </c>
+      <c r="N16" t="s">
+        <v>99</v>
+      </c>
+      <c r="O16" t="s">
+        <v>100</v>
+      </c>
+      <c r="P16" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" t="s">
+        <v>108</v>
+      </c>
+      <c r="N17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
complete half first of admin menu
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\Codegym_Module_2\Case_Study\accounting_software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE29DE3-D692-45AE-B5B2-DF7D2EF5BE7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F0CE60-4342-4B21-BE24-0FD8F6283E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{97F2DD4E-FD07-4A13-BFEB-826D5C26E65D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{97F2DD4E-FD07-4A13-BFEB-826D5C26E65D}"/>
   </bookViews>
   <sheets>
     <sheet name="idea" sheetId="1" r:id="rId1"/>
     <sheet name="shortVersion" sheetId="2" r:id="rId2"/>
     <sheet name="156" sheetId="3" r:id="rId3"/>
+    <sheet name="Menu" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="150">
   <si>
     <t>Tiền mặt</t>
   </si>
@@ -354,6 +355,129 @@
   </si>
   <si>
     <t>hàng hỏng/ lý do khác</t>
+  </si>
+  <si>
+    <t>Run</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>&gt;login</t>
+  </si>
+  <si>
+    <t>&gt;Admin</t>
+  </si>
+  <si>
+    <t>&gt;Show product</t>
+  </si>
+  <si>
+    <t>&gt;Show all</t>
+  </si>
+  <si>
+    <t>&gt;Show Limited</t>
+  </si>
+  <si>
+    <t>&gt;Show unlimited</t>
+  </si>
+  <si>
+    <t>&gt;sort by</t>
+  </si>
+  <si>
+    <t>&gt;Create note</t>
+  </si>
+  <si>
+    <t>&gt;receive note</t>
+  </si>
+  <si>
+    <t>&gt;delivery note</t>
+  </si>
+  <si>
+    <t>&gt;Remove product</t>
+  </si>
+  <si>
+    <t>&gt;Find Product</t>
+  </si>
+  <si>
+    <t>&gt;Business Manager</t>
+  </si>
+  <si>
+    <t>&gt;Product Manager</t>
+  </si>
+  <si>
+    <t>&gt;Show note list</t>
+  </si>
+  <si>
+    <t>&gt;calculate</t>
+  </si>
+  <si>
+    <t>&gt;back to previous</t>
+  </si>
+  <si>
+    <t>&gt;Back to previous</t>
+  </si>
+  <si>
+    <t>&gt;show receive note</t>
+  </si>
+  <si>
+    <t>&gt;show delivery note</t>
+  </si>
+  <si>
+    <t>&gt;add money</t>
+  </si>
+  <si>
+    <t>&gt;User manager</t>
+  </si>
+  <si>
+    <t>&gt;find note</t>
+  </si>
+  <si>
+    <t>&gt;show user list</t>
+  </si>
+  <si>
+    <t>&gt;show all</t>
+  </si>
+  <si>
+    <t>&gt;show accountant</t>
+  </si>
+  <si>
+    <t>&gt;show store keeper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;show sale staff </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;create new user </t>
+  </si>
+  <si>
+    <t>&gt;accountant</t>
+  </si>
+  <si>
+    <t>&gt;storekeeper</t>
+  </si>
+  <si>
+    <t>&gt;salestaff</t>
+  </si>
+  <si>
+    <t>&gt;remove user</t>
+  </si>
+  <si>
+    <t>&gt;find user</t>
+  </si>
+  <si>
+    <t>&gt;Accountant</t>
+  </si>
+  <si>
+    <t>&gt;Storekeeper</t>
+  </si>
+  <si>
+    <t>&gt;SaleStaff</t>
+  </si>
+  <si>
+    <t>&gt;Log out</t>
+  </si>
+  <si>
+    <t>&gt;exit</t>
   </si>
 </sst>
 </file>
@@ -1255,7 +1379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2859D1AD-D06B-4526-AF9E-F8462D477E43}">
   <dimension ref="B5:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -1440,4 +1564,425 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{439AC360-CDEB-459F-9D40-2C9A13DABBCA}">
+  <dimension ref="A2:G74"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>122</v>
+      </c>
+      <c r="F10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>123</v>
+      </c>
+      <c r="E14" t="s">
+        <v>125</v>
+      </c>
+      <c r="F14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>132</v>
+      </c>
+      <c r="E23" t="s">
+        <v>134</v>
+      </c>
+      <c r="F23" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="F24" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="F25" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="F26" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="27" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="F27" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="E28" t="s">
+        <v>139</v>
+      </c>
+      <c r="F28" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="29" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="F29" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="F30" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="31" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="F31" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="E32" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E33" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E34" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>145</v>
+      </c>
+      <c r="D37" t="s">
+        <v>113</v>
+      </c>
+      <c r="E37" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E38" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E39" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E40" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D42" t="s">
+        <v>125</v>
+      </c>
+      <c r="E42" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E43" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E44" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E45" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D46" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D47" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D48" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>146</v>
+      </c>
+      <c r="D50" t="s">
+        <v>113</v>
+      </c>
+      <c r="E50" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E51" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E52" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="53" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E53" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E54" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="55" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D55" t="s">
+        <v>118</v>
+      </c>
+      <c r="E55" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="56" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E56" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E57" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="58" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D58" t="s">
+        <v>122</v>
+      </c>
+      <c r="E58" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E59" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="60" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D60" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="62" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C62" t="s">
+        <v>147</v>
+      </c>
+      <c r="D62" t="s">
+        <v>113</v>
+      </c>
+      <c r="E62" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="63" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E63" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="64" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E64" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E65" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D67" t="s">
+        <v>118</v>
+      </c>
+      <c r="E67" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D68" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D69" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D70" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C72" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed drawn business result format/ Need fix the logic bug of calculate business result
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,27 +8,39 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\Codegym_Module_2\Case_Study\accounting_software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F0CE60-4342-4B21-BE24-0FD8F6283E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3DD1B8-E8E1-422E-9369-79E0DB042CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{97F2DD4E-FD07-4A13-BFEB-826D5C26E65D}"/>
+    <workbookView xWindow="11508" yWindow="0" windowWidth="11328" windowHeight="11964" activeTab="4" xr2:uid="{97F2DD4E-FD07-4A13-BFEB-826D5C26E65D}"/>
   </bookViews>
   <sheets>
     <sheet name="idea" sheetId="1" r:id="rId1"/>
     <sheet name="shortVersion" sheetId="2" r:id="rId2"/>
     <sheet name="156" sheetId="3" r:id="rId3"/>
     <sheet name="Menu" sheetId="4" r:id="rId4"/>
+    <sheet name="Test_Script" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="168">
   <si>
     <t>Tiền mặt</t>
   </si>
@@ -478,13 +490,67 @@
   </si>
   <si>
     <t>&gt;exit</t>
+  </si>
+  <si>
+    <t>stt</t>
+  </si>
+  <si>
+    <t>Tên hàng</t>
+  </si>
+  <si>
+    <t>San pham thu nghiem 1</t>
+  </si>
+  <si>
+    <t>Nhập kho</t>
+  </si>
+  <si>
+    <t>San pham thu nghiem 2</t>
+  </si>
+  <si>
+    <t>Giá nhập</t>
+  </si>
+  <si>
+    <t>Giá bán</t>
+  </si>
+  <si>
+    <t>San pham thu nghiem 3</t>
+  </si>
+  <si>
+    <t>Tổng giá vốn</t>
+  </si>
+  <si>
+    <t>Tổng số lượng</t>
+  </si>
+  <si>
+    <t>Tổng thu nhập(nếu bán hết)</t>
+  </si>
+  <si>
+    <t>Xuất kho</t>
+  </si>
+  <si>
+    <t>Số lượng bán</t>
+  </si>
+  <si>
+    <t>Tổng thu về</t>
+  </si>
+  <si>
+    <t>Giá vốn</t>
+  </si>
+  <si>
+    <t>"= 100*10 + 60*10+120*10</t>
+  </si>
+  <si>
+    <t>"= 200*20 + 250*5</t>
+  </si>
+  <si>
+    <t>"=5*300</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,16 +573,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -539,11 +623,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -552,6 +682,57 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1570,7 +1751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{439AC360-CDEB-459F-9D40-2C9A13DABBCA}">
   <dimension ref="A2:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -1985,4 +2166,406 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A24E2DE-9A7D-4230-A0E4-6CD395786926}">
+  <dimension ref="A1:L15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="8"/>
+    <col min="2" max="2" width="20" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" style="8" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="8"/>
+    <col min="6" max="6" width="22.6640625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" style="8" customWidth="1"/>
+    <col min="8" max="8" width="10.21875" style="8" customWidth="1"/>
+    <col min="9" max="9" width="28.33203125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" style="8" customWidth="1"/>
+    <col min="11" max="11" width="18.44140625" style="8" customWidth="1"/>
+    <col min="12" max="12" width="11.21875" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="1:12" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="G2" s="11"/>
+      <c r="H2" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="14">
+        <v>10</v>
+      </c>
+      <c r="D3" s="9">
+        <v>100</v>
+      </c>
+      <c r="E3" s="9">
+        <v>150</v>
+      </c>
+      <c r="F3" s="15">
+        <f>C3*D3</f>
+        <v>1000</v>
+      </c>
+      <c r="G3" s="16"/>
+      <c r="H3" s="9">
+        <f>E3*C3</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="9">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" s="9">
+        <v>20</v>
+      </c>
+      <c r="D4" s="9">
+        <v>200</v>
+      </c>
+      <c r="E4" s="9">
+        <v>300</v>
+      </c>
+      <c r="F4" s="17">
+        <f>C4*D4</f>
+        <v>4000</v>
+      </c>
+      <c r="G4" s="18"/>
+      <c r="H4" s="9">
+        <f>E4*C4</f>
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="9">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5" s="9">
+        <v>30</v>
+      </c>
+      <c r="D5" s="9">
+        <v>300</v>
+      </c>
+      <c r="E5" s="9">
+        <v>500</v>
+      </c>
+      <c r="F5" s="17">
+        <f>C5*D5</f>
+        <v>9000</v>
+      </c>
+      <c r="G5" s="18"/>
+      <c r="H5" s="9">
+        <f>E5*C5</f>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="9">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="14">
+        <v>10</v>
+      </c>
+      <c r="D6" s="9">
+        <v>60</v>
+      </c>
+      <c r="E6" s="9">
+        <v>150</v>
+      </c>
+      <c r="F6" s="15">
+        <f>C6*D6</f>
+        <v>600</v>
+      </c>
+      <c r="G6" s="16"/>
+      <c r="H6" s="9">
+        <f>E6*C6</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="9">
+        <v>5</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="14">
+        <v>10</v>
+      </c>
+      <c r="D7" s="9">
+        <v>120</v>
+      </c>
+      <c r="E7" s="9">
+        <v>150</v>
+      </c>
+      <c r="F7" s="15">
+        <f>C7*D7</f>
+        <v>1200</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="9">
+        <f>E7*C7</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="9">
+        <v>6</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C8" s="19">
+        <v>10</v>
+      </c>
+      <c r="D8" s="9">
+        <v>250</v>
+      </c>
+      <c r="E8" s="9">
+        <v>300</v>
+      </c>
+      <c r="F8" s="20">
+        <f>C8*D8</f>
+        <v>2500</v>
+      </c>
+      <c r="G8" s="21"/>
+      <c r="H8" s="9">
+        <f>E8*C8</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+    </row>
+    <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="9">
+        <v>1</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C12" s="9">
+        <v>30</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9">
+        <v>150</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="G12" s="9">
+        <f>100*10+60*10+120*10</f>
+        <v>2800</v>
+      </c>
+      <c r="H12" s="9">
+        <f>C12*E12</f>
+        <v>4500</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="K12" s="9">
+        <v>30</v>
+      </c>
+      <c r="L12" s="9">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="9">
+        <v>2</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C13" s="9">
+        <v>25</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9">
+        <v>300</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="G13" s="9">
+        <f>20*200+250*5</f>
+        <v>5250</v>
+      </c>
+      <c r="H13" s="9">
+        <f>C13*E13</f>
+        <v>7500</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="K13" s="9">
+        <v>30</v>
+      </c>
+      <c r="L13" s="9">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="9">
+        <v>3</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C14" s="9">
+        <v>5</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9">
+        <v>500</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="G14" s="9">
+        <f>300*5</f>
+        <v>1500</v>
+      </c>
+      <c r="H14" s="9">
+        <f>C14*E14</f>
+        <v>2500</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="K14" s="9">
+        <v>30</v>
+      </c>
+      <c r="L14" s="9">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="9">
+        <v>4</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9">
+        <f>SUM(G12:G14)</f>
+        <v>9550</v>
+      </c>
+      <c r="H15" s="9">
+        <f>SUM(H12:H14)</f>
+        <v>14500</v>
+      </c>
+      <c r="I15" s="8">
+        <f>H15-G15</f>
+        <v>4950</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix and update Load save file (NoteList)
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\Codegym_Module_2\Case_Study\accounting_software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3DD1B8-E8E1-422E-9369-79E0DB042CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9563D75A-ABA7-47C2-A998-AAC32D578C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11508" yWindow="0" windowWidth="11328" windowHeight="11964" activeTab="4" xr2:uid="{97F2DD4E-FD07-4A13-BFEB-826D5C26E65D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="4" xr2:uid="{97F2DD4E-FD07-4A13-BFEB-826D5C26E65D}"/>
   </bookViews>
   <sheets>
     <sheet name="idea" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="182">
   <si>
     <t>Tiền mặt</t>
   </si>
@@ -544,6 +544,48 @@
   </si>
   <si>
     <t>"=5*300</t>
+  </si>
+  <si>
+    <t>Kịch bản Test</t>
+  </si>
+  <si>
+    <t>Đăng nhập admin</t>
+  </si>
+  <si>
+    <t>check user</t>
+  </si>
+  <si>
+    <t>show note</t>
+  </si>
+  <si>
+    <t>clear note</t>
+  </si>
+  <si>
+    <t>Đăng nhập thủ kho</t>
+  </si>
+  <si>
+    <t>Tạo phiếu nhập kho</t>
+  </si>
+  <si>
+    <t>Đăng nhập nv bán hàng</t>
+  </si>
+  <si>
+    <t>Tạo phiếu xuất kho</t>
+  </si>
+  <si>
+    <t>Show sản phẩm</t>
+  </si>
+  <si>
+    <t>Đăng nhập kết toán</t>
+  </si>
+  <si>
+    <t>Show kết quả kinh doanh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Show sản phẩm ( hết hàng out of stock)</t>
   </si>
 </sst>
 </file>
@@ -673,7 +715,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -682,32 +724,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -721,17 +763,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2170,391 +2215,481 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A24E2DE-9A7D-4230-A0E4-6CD395786926}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="8"/>
-    <col min="2" max="2" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" style="8" customWidth="1"/>
-    <col min="4" max="5" width="8.88671875" style="8"/>
-    <col min="6" max="6" width="22.6640625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" style="8" customWidth="1"/>
-    <col min="8" max="8" width="10.21875" style="8" customWidth="1"/>
-    <col min="9" max="9" width="28.33203125" style="8" customWidth="1"/>
-    <col min="10" max="10" width="22.33203125" style="8" customWidth="1"/>
-    <col min="11" max="11" width="18.44140625" style="8" customWidth="1"/>
-    <col min="12" max="12" width="11.21875" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="8"/>
+    <col min="1" max="1" width="5.109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="20" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" style="6" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="6"/>
+    <col min="6" max="6" width="22.6640625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" style="6" customWidth="1"/>
+    <col min="8" max="8" width="10.21875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="28.33203125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="18.44140625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="11.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:12" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12" t="s">
+      <c r="G2" s="14"/>
+      <c r="H2" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="9">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="8">
         <v>10</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="7">
         <v>100</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="7">
         <v>150</v>
       </c>
       <c r="F3" s="15">
-        <f>C3*D3</f>
+        <f t="shared" ref="F3:F8" si="0">C3*D3</f>
         <v>1000</v>
       </c>
       <c r="G3" s="16"/>
-      <c r="H3" s="9">
-        <f>E3*C3</f>
+      <c r="H3" s="7">
+        <f t="shared" ref="H3:H8" si="1">E3*C3</f>
         <v>1500</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="9">
+      <c r="A4" s="7">
         <v>2</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="7">
         <v>20</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="7">
         <v>200</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="7">
         <v>300</v>
       </c>
       <c r="F4" s="17">
-        <f>C4*D4</f>
+        <f t="shared" si="0"/>
         <v>4000</v>
       </c>
       <c r="G4" s="18"/>
-      <c r="H4" s="9">
-        <f>E4*C4</f>
+      <c r="H4" s="7">
+        <f t="shared" si="1"/>
         <v>6000</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="9">
+      <c r="A5" s="7">
         <v>3</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="7">
         <v>30</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="7">
         <v>300</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="7">
         <v>500</v>
       </c>
       <c r="F5" s="17">
-        <f>C5*D5</f>
+        <f t="shared" si="0"/>
         <v>9000</v>
       </c>
       <c r="G5" s="18"/>
-      <c r="H5" s="9">
-        <f>E5*C5</f>
+      <c r="H5" s="7">
+        <f t="shared" si="1"/>
         <v>15000</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="9">
+      <c r="A6" s="7">
         <v>4</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="8">
         <v>10</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="7">
         <v>60</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="7">
         <v>150</v>
       </c>
       <c r="F6" s="15">
-        <f>C6*D6</f>
+        <f t="shared" si="0"/>
         <v>600</v>
       </c>
       <c r="G6" s="16"/>
-      <c r="H6" s="9">
-        <f>E6*C6</f>
+      <c r="H6" s="7">
+        <f t="shared" si="1"/>
         <v>1500</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="9">
+      <c r="A7" s="7">
         <v>5</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="8">
         <v>10</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="7">
         <v>120</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="7">
         <v>150</v>
       </c>
       <c r="F7" s="15">
-        <f>C7*D7</f>
+        <f t="shared" si="0"/>
         <v>1200</v>
       </c>
       <c r="G7" s="16"/>
-      <c r="H7" s="9">
-        <f>E7*C7</f>
+      <c r="H7" s="7">
+        <f t="shared" si="1"/>
         <v>1500</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="9">
+      <c r="A8" s="7">
         <v>6</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="9">
         <v>10</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="7">
         <v>250</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="7">
         <v>300</v>
       </c>
-      <c r="F8" s="20">
-        <f>C8*D8</f>
+      <c r="F8" s="19">
+        <f t="shared" si="0"/>
         <v>2500</v>
       </c>
-      <c r="G8" s="21"/>
-      <c r="H8" s="9">
-        <f>E8*C8</f>
+      <c r="G8" s="20"/>
+      <c r="H8" s="7">
+        <f t="shared" si="1"/>
         <v>3000</v>
       </c>
     </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B9" s="6"/>
+    </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9" t="s">
+      <c r="D11" s="7"/>
+      <c r="E11" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9" t="s">
+      <c r="F11" s="7"/>
+      <c r="G11" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9" t="s">
+      <c r="J11" s="7"/>
+      <c r="K11" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="L11" s="9" t="s">
+      <c r="L11" s="7" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="9">
+      <c r="A12" s="7">
         <v>1</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="7">
         <v>30</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9">
+      <c r="D12" s="7"/>
+      <c r="E12" s="7">
         <v>150</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="7">
         <f>100*10+60*10+120*10</f>
         <v>2800</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="7">
         <f>C12*E12</f>
         <v>4500</v>
       </c>
-      <c r="J12" s="9" t="s">
+      <c r="J12" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="K12" s="9">
+      <c r="K12" s="7">
         <v>30</v>
       </c>
-      <c r="L12" s="9">
+      <c r="L12" s="7">
         <v>2800</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="9">
+      <c r="A13" s="7">
         <v>2</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="7">
         <v>25</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9">
+      <c r="D13" s="7"/>
+      <c r="E13" s="7">
         <v>300</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="7">
         <f>20*200+250*5</f>
         <v>5250</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="7">
         <f>C13*E13</f>
         <v>7500</v>
       </c>
-      <c r="J13" s="9" t="s">
+      <c r="J13" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="K13" s="9">
+      <c r="K13" s="7">
         <v>30</v>
       </c>
-      <c r="L13" s="9">
+      <c r="L13" s="7">
         <v>6500</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="9">
+      <c r="A14" s="7">
         <v>3</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="7">
         <v>5</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9">
+      <c r="D14" s="7"/>
+      <c r="E14" s="7">
         <v>500</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="7">
         <f>300*5</f>
         <v>1500</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="7">
         <f>C14*E14</f>
         <v>2500</v>
       </c>
-      <c r="J14" s="9" t="s">
+      <c r="J14" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="K14" s="9">
+      <c r="K14" s="7">
         <v>30</v>
       </c>
-      <c r="L14" s="9">
+      <c r="L14" s="7">
         <v>9000</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="9">
+      <c r="A15" s="7">
         <v>4</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7">
         <f>SUM(G12:G14)</f>
         <v>9550</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="7">
         <f>SUM(H12:H14)</f>
         <v>14500</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="6">
         <f>H15-G15</f>
         <v>4950</v>
       </c>
     </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="B18" s="22"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="23">
+        <v>1</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C20" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C21" s="6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C22" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B23" s="23">
+        <v>2</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C24" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B26" s="23">
+        <v>3</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C27" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C28" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C29" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B31" s="23">
+        <v>4</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C32" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="A18:B18"/>
     <mergeCell ref="A10:H10"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="F2:G2"/>

</xml_diff>